<commit_message>
search box searches entire company object not just name
The Boeing company —> boeing
The Nielsen company —> nielsen, id is still nielco (fixed typo)
got rid of misplaced files
tried to add an industry search filter but haven’t called it yet
</commit_message>
<xml_diff>
--- a/reference/iday14-supplementary-data.xlsx
+++ b/reference/iday14-supplementary-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28720" windowHeight="17560" tabRatio="500" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="linkedinnumtoname" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7327" uniqueCount="2154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7448" uniqueCount="2154">
   <si>
     <t>csoorgname</t>
   </si>
@@ -6495,7 +6495,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6555,6 +6555,13 @@
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -6621,7 +6628,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="287">
+  <cellStyleXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6909,8 +6916,88 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -6960,8 +7047,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="287">
+  <cellStyles count="367">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -7105,6 +7196,46 @@
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -7247,6 +7378,46 @@
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="12"/>
   </cellStyles>
@@ -7577,21 +7748,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="6"/>
+    <col min="4" max="4" width="10.83203125" style="6"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>666</v>
       </c>
@@ -7602,8 +7777,17 @@
         <v>668</v>
       </c>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="15">
+      <c r="E1" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>668</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="7">
         <v>1864</v>
       </c>
@@ -7613,11 +7797,20 @@
       <c r="C2" s="6" t="s">
         <v>669</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="E2">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>669</v>
+      </c>
+      <c r="G2" s="7">
+        <v>1864</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:10">
       <c r="A3" s="7">
         <v>3601307</v>
       </c>
@@ -7627,11 +7820,20 @@
       <c r="C3" s="6" t="s">
         <v>671</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="E3">
+        <v>1551</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>671</v>
+      </c>
+      <c r="G3" s="7">
+        <v>3601307</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:10">
       <c r="A4" s="7">
         <v>211674</v>
       </c>
@@ -7641,11 +7843,20 @@
       <c r="C4" s="6" t="s">
         <v>673</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="E4">
+        <v>1240</v>
+      </c>
+      <c r="F4" t="s">
+        <v>673</v>
+      </c>
+      <c r="G4" s="7">
+        <v>211674</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:10">
       <c r="A5" s="7">
         <v>1058</v>
       </c>
@@ -7655,11 +7866,20 @@
       <c r="C5" s="6" t="s">
         <v>675</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="E5">
+        <v>373</v>
+      </c>
+      <c r="F5" t="s">
+        <v>675</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1058</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:10">
       <c r="A6" s="7">
         <v>1835</v>
       </c>
@@ -7669,11 +7889,20 @@
       <c r="C6" s="6" t="s">
         <v>678</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="E6">
+        <v>396</v>
+      </c>
+      <c r="F6" t="s">
+        <v>678</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1835</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:10">
       <c r="A7" s="7">
         <v>1052</v>
       </c>
@@ -7683,11 +7912,20 @@
       <c r="C7" s="6" t="s">
         <v>680</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="E7">
+        <v>1530</v>
+      </c>
+      <c r="F7" t="s">
+        <v>680</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1052</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15">
+    <row r="8" spans="1:10">
       <c r="A8" s="7" t="s">
         <v>682</v>
       </c>
@@ -7695,11 +7933,16 @@
         <v>20</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="I8" s="6" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="23" t="s">
+        <v>682</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:10">
       <c r="A9" s="7">
         <v>2371</v>
       </c>
@@ -7709,8 +7952,17 @@
       <c r="C9" s="6" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15">
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>685</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="7">
         <v>1266312</v>
       </c>
@@ -7720,8 +7972,17 @@
       <c r="C10" s="6" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15">
+      <c r="E10">
+        <v>1069</v>
+      </c>
+      <c r="F10" t="s">
+        <v>686</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1266312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="7">
         <v>17427</v>
       </c>
@@ -7731,8 +7992,17 @@
       <c r="C11" s="6" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15">
+      <c r="E11">
+        <v>480</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>757</v>
+      </c>
+      <c r="G11" s="23">
+        <v>17427</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="11">
         <v>233024</v>
       </c>
@@ -7742,8 +8012,17 @@
       <c r="C12" s="6" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15">
+      <c r="E12">
+        <v>1160</v>
+      </c>
+      <c r="F12" t="s">
+        <v>689</v>
+      </c>
+      <c r="G12" s="11">
+        <v>233024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="7">
         <v>1616</v>
       </c>
@@ -7753,11 +8032,20 @@
       <c r="C13" s="6" t="s">
         <v>691</v>
       </c>
-      <c r="H13" s="6">
+      <c r="E13">
+        <v>930</v>
+      </c>
+      <c r="F13" t="s">
+        <v>691</v>
+      </c>
+      <c r="G13" s="7">
         <v>1616</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15">
+      <c r="I13" s="6">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="7">
         <v>48775</v>
       </c>
@@ -7767,8 +8055,17 @@
       <c r="C14" s="6" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15">
+      <c r="E14">
+        <v>1285</v>
+      </c>
+      <c r="F14" t="s">
+        <v>692</v>
+      </c>
+      <c r="G14" s="7">
+        <v>48775</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="7">
         <v>5499</v>
       </c>
@@ -7778,8 +8075,17 @@
       <c r="C15" s="6" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15">
+      <c r="E15">
+        <v>1026</v>
+      </c>
+      <c r="F15" t="s">
+        <v>693</v>
+      </c>
+      <c r="G15" s="7">
+        <v>5499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="7">
         <v>3762</v>
       </c>
@@ -7789,8 +8095,17 @@
       <c r="C16" s="6" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15">
+      <c r="E16">
+        <v>622</v>
+      </c>
+      <c r="F16" t="s">
+        <v>695</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="7">
         <v>670584</v>
       </c>
@@ -7800,8 +8115,17 @@
       <c r="C17" s="6" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15">
+      <c r="E17">
+        <v>1227</v>
+      </c>
+      <c r="F17" t="s">
+        <v>697</v>
+      </c>
+      <c r="G17" s="7">
+        <v>670584</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="7">
         <v>163658</v>
       </c>
@@ -7811,11 +8135,20 @@
       <c r="C18" s="6" t="s">
         <v>699</v>
       </c>
-      <c r="H18" s="6">
+      <c r="E18">
+        <v>852</v>
+      </c>
+      <c r="F18" t="s">
+        <v>699</v>
+      </c>
+      <c r="G18" s="7">
         <v>163658</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15">
+      <c r="I18" s="6">
+        <v>163658</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="7">
         <v>1689</v>
       </c>
@@ -7825,8 +8158,17 @@
       <c r="C19" s="6" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15">
+      <c r="E19">
+        <v>437</v>
+      </c>
+      <c r="F19" t="s">
+        <v>701</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="7">
         <v>1483</v>
       </c>
@@ -7836,8 +8178,17 @@
       <c r="C20" s="6" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15">
+      <c r="E20">
+        <v>118</v>
+      </c>
+      <c r="F20" t="s">
+        <v>703</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="7">
         <v>10809</v>
       </c>
@@ -7847,8 +8198,17 @@
       <c r="C21" s="6" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15">
+      <c r="E21">
+        <v>632</v>
+      </c>
+      <c r="F21" t="s">
+        <v>704</v>
+      </c>
+      <c r="G21" s="7">
+        <v>10809</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="7">
         <v>9170</v>
       </c>
@@ -7858,8 +8218,17 @@
       <c r="C22" s="6" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15">
+      <c r="E22">
+        <v>1074</v>
+      </c>
+      <c r="F22" t="s">
+        <v>705</v>
+      </c>
+      <c r="G22" s="7">
+        <v>9170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="7" t="s">
         <v>682</v>
       </c>
@@ -7867,8 +8236,15 @@
         <v>58</v>
       </c>
       <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" ht="15">
+      <c r="E23" s="16">
+        <v>336</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="23" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="7">
         <v>1015</v>
       </c>
@@ -7878,8 +8254,14 @@
       <c r="C24" s="6" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15">
+      <c r="F24" t="s">
+        <v>707</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="7">
         <v>3915</v>
       </c>
@@ -7889,8 +8271,17 @@
       <c r="C25" s="6" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15">
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>708</v>
+      </c>
+      <c r="G25" s="7">
+        <v>3915</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="7">
         <v>1441</v>
       </c>
@@ -7900,8 +8291,17 @@
       <c r="C26" s="6" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15">
+      <c r="E26">
+        <v>922</v>
+      </c>
+      <c r="F26" t="s">
+        <v>710</v>
+      </c>
+      <c r="G26" s="7">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="7">
         <v>355611</v>
       </c>
@@ -7911,8 +8311,17 @@
       <c r="C27" s="6" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15">
+      <c r="E27">
+        <v>1143</v>
+      </c>
+      <c r="F27" t="s">
+        <v>712</v>
+      </c>
+      <c r="G27" s="7">
+        <v>355611</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="7">
         <v>91563</v>
       </c>
@@ -7922,8 +8331,17 @@
       <c r="C28" s="6" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15">
+      <c r="E28">
+        <v>1305</v>
+      </c>
+      <c r="F28" t="s">
+        <v>714</v>
+      </c>
+      <c r="G28" s="7">
+        <v>91563</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="7">
         <v>3237134</v>
       </c>
@@ -7933,8 +8351,17 @@
       <c r="C29" s="6" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15">
+      <c r="E29">
+        <v>1729</v>
+      </c>
+      <c r="F29" t="s">
+        <v>715</v>
+      </c>
+      <c r="G29" s="7">
+        <v>3237134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="7">
         <v>11204</v>
       </c>
@@ -7944,8 +8371,17 @@
       <c r="C30" s="6" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15">
+      <c r="E30">
+        <v>1580</v>
+      </c>
+      <c r="F30" t="s">
+        <v>717</v>
+      </c>
+      <c r="G30" s="7">
+        <v>11204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="7">
         <v>40620</v>
       </c>
@@ -7955,8 +8391,17 @@
       <c r="C31" s="6" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15">
+      <c r="E31">
+        <v>1255</v>
+      </c>
+      <c r="F31" t="s">
+        <v>719</v>
+      </c>
+      <c r="G31" s="7">
+        <v>40620</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="7">
         <v>90985</v>
       </c>
@@ -7966,8 +8411,17 @@
       <c r="C32" s="6" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15">
+      <c r="E32">
+        <v>1076</v>
+      </c>
+      <c r="F32" t="s">
+        <v>722</v>
+      </c>
+      <c r="G32" s="7">
+        <v>90985</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="7">
         <v>2670814</v>
       </c>
@@ -7977,8 +8431,17 @@
       <c r="C33" s="6" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15">
+      <c r="E33">
+        <v>1814</v>
+      </c>
+      <c r="F33" t="s">
+        <v>723</v>
+      </c>
+      <c r="G33" s="7">
+        <v>2670814</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="7">
         <v>11670</v>
       </c>
@@ -7988,8 +8451,17 @@
       <c r="C34" s="6" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15">
+      <c r="E34">
+        <v>717</v>
+      </c>
+      <c r="F34" t="s">
+        <v>724</v>
+      </c>
+      <c r="G34" s="7">
+        <v>11670</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="7">
         <v>9652</v>
       </c>
@@ -7999,8 +8471,17 @@
       <c r="C35" s="6" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="15">
+      <c r="E35">
+        <v>1229</v>
+      </c>
+      <c r="F35" t="s">
+        <v>725</v>
+      </c>
+      <c r="G35" s="7">
+        <v>9652</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="7">
         <v>2247</v>
       </c>
@@ -8010,8 +8491,17 @@
       <c r="C36" s="6" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="15">
+      <c r="E36">
+        <v>1628</v>
+      </c>
+      <c r="F36" t="s">
+        <v>727</v>
+      </c>
+      <c r="G36" s="7">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="11">
         <v>75160</v>
       </c>
@@ -8021,8 +8511,17 @@
       <c r="C37" s="6" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15">
+      <c r="E37">
+        <v>525</v>
+      </c>
+      <c r="F37" t="s">
+        <v>728</v>
+      </c>
+      <c r="G37" s="11">
+        <v>75160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="11">
         <v>9585</v>
       </c>
@@ -8032,11 +8531,20 @@
       <c r="C38" s="6" t="s">
         <v>728</v>
       </c>
-      <c r="H38" s="6">
+      <c r="E38">
+        <v>999</v>
+      </c>
+      <c r="F38" t="s">
+        <v>731</v>
+      </c>
+      <c r="G38" s="11">
         <v>9585</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="15">
+      <c r="I38" s="6">
+        <v>9585</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="11">
         <v>1194036</v>
       </c>
@@ -8046,11 +8554,20 @@
       <c r="C39" s="6" t="s">
         <v>729</v>
       </c>
-      <c r="H39" s="6">
+      <c r="E39">
+        <v>475</v>
+      </c>
+      <c r="F39" t="s">
+        <v>733</v>
+      </c>
+      <c r="G39" s="11">
         <v>1194036</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15">
+      <c r="I39" s="6">
+        <v>1194036</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="11">
         <v>47117</v>
       </c>
@@ -8060,8 +8577,17 @@
       <c r="C40" s="6" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="15">
+      <c r="E40">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>734</v>
+      </c>
+      <c r="G40" s="23">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="11">
         <v>403579</v>
       </c>
@@ -8071,8 +8597,17 @@
       <c r="C41" s="6" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="15">
+      <c r="E41">
+        <v>1084</v>
+      </c>
+      <c r="F41" t="s">
+        <v>737</v>
+      </c>
+      <c r="G41" s="11">
+        <v>47117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="11">
         <v>1035</v>
       </c>
@@ -8082,8 +8617,11 @@
       <c r="C42" s="6" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15">
+      <c r="G42" s="11">
+        <v>403579</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="11">
         <v>1771432</v>
       </c>
@@ -8093,8 +8631,17 @@
       <c r="C43" s="6" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="15">
+      <c r="E43">
+        <v>17</v>
+      </c>
+      <c r="F43" t="s">
+        <v>736</v>
+      </c>
+      <c r="G43" s="23">
+        <v>1771432</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="11">
         <v>870904</v>
       </c>
@@ -8104,8 +8651,17 @@
       <c r="C44" s="6" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="15">
+      <c r="E44">
+        <v>972</v>
+      </c>
+      <c r="F44" t="s">
+        <v>759</v>
+      </c>
+      <c r="G44" s="11">
+        <v>870904</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="11">
         <v>2445</v>
       </c>
@@ -8115,8 +8671,17 @@
       <c r="C45" s="6" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="15">
+      <c r="E45">
+        <v>1575</v>
+      </c>
+      <c r="F45" t="s">
+        <v>738</v>
+      </c>
+      <c r="G45" s="11">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="11">
         <v>5169</v>
       </c>
@@ -8126,8 +8691,17 @@
       <c r="C46" s="6" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="15">
+      <c r="E46">
+        <v>1798</v>
+      </c>
+      <c r="F46" t="s">
+        <v>739</v>
+      </c>
+      <c r="G46" s="11">
+        <v>5169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="11">
         <v>18355</v>
       </c>
@@ -8137,8 +8711,17 @@
       <c r="C47" s="6" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="15">
+      <c r="E47">
+        <v>1000</v>
+      </c>
+      <c r="F47" t="s">
+        <v>741</v>
+      </c>
+      <c r="G47" s="11">
+        <v>18355</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="11">
         <v>1431</v>
       </c>
@@ -8148,8 +8731,17 @@
       <c r="C48" s="6" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15">
+      <c r="E48">
+        <v>572</v>
+      </c>
+      <c r="F48" t="s">
+        <v>743</v>
+      </c>
+      <c r="G48" s="11">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="12">
         <v>2425</v>
       </c>
@@ -8159,8 +8751,17 @@
       <c r="C49" s="6" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15">
+      <c r="E49">
+        <v>495</v>
+      </c>
+      <c r="F49" t="s">
+        <v>745</v>
+      </c>
+      <c r="G49" s="12">
+        <v>2425</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="11">
         <v>1116</v>
       </c>
@@ -8170,8 +8771,17 @@
       <c r="C50" s="6" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="15">
+      <c r="E50">
+        <v>117</v>
+      </c>
+      <c r="F50" t="s">
+        <v>747</v>
+      </c>
+      <c r="G50" s="11">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="11">
         <v>60540</v>
       </c>
@@ -8181,8 +8791,17 @@
       <c r="C51" s="6" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15">
+      <c r="E51">
+        <v>1826</v>
+      </c>
+      <c r="F51" t="s">
+        <v>748</v>
+      </c>
+      <c r="G51" s="11">
+        <v>60540</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="14">
         <v>165806</v>
       </c>
@@ -8192,8 +8811,17 @@
       <c r="C52" s="6" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15">
+      <c r="E52">
+        <v>172</v>
+      </c>
+      <c r="F52" t="s">
+        <v>750</v>
+      </c>
+      <c r="G52" s="14">
+        <v>165806</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="11">
         <v>157241</v>
       </c>
@@ -8203,8 +8831,17 @@
       <c r="C53" s="6" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15">
+      <c r="E53">
+        <v>485</v>
+      </c>
+      <c r="F53" t="s">
+        <v>752</v>
+      </c>
+      <c r="G53" s="11">
+        <v>157241</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="11">
         <v>85802</v>
       </c>
@@ -8214,8 +8851,17 @@
       <c r="C54" s="6" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15">
+      <c r="E54">
+        <v>1248</v>
+      </c>
+      <c r="F54" t="s">
+        <v>753</v>
+      </c>
+      <c r="G54" s="11">
+        <v>85802</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="11">
         <v>155480</v>
       </c>
@@ -8225,8 +8871,17 @@
       <c r="C55" s="6" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15">
+      <c r="E55">
+        <v>1272</v>
+      </c>
+      <c r="F55" t="s">
+        <v>755</v>
+      </c>
+      <c r="G55" s="11">
+        <v>155480</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="11">
         <v>1384</v>
       </c>
@@ -8236,8 +8891,11 @@
       <c r="C56" s="6" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="15">
+      <c r="G56" s="11">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="11">
         <v>1714</v>
       </c>
@@ -8247,8 +8905,17 @@
       <c r="C57" s="6" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="15">
+      <c r="E57">
+        <v>1274</v>
+      </c>
+      <c r="F57" t="s">
+        <v>729</v>
+      </c>
+      <c r="G57" s="11">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="7">
         <v>157356</v>
       </c>
@@ -8258,8 +8925,17 @@
       <c r="C58" s="6" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="15">
+      <c r="E58">
+        <v>1070</v>
+      </c>
+      <c r="F58" t="s">
+        <v>760</v>
+      </c>
+      <c r="G58" s="7">
+        <v>157356</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="7">
         <v>1335</v>
       </c>
@@ -8269,8 +8945,17 @@
       <c r="C59" s="6" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="15">
+      <c r="E59">
+        <v>1325</v>
+      </c>
+      <c r="F59" t="s">
+        <v>762</v>
+      </c>
+      <c r="G59" s="7">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="7">
         <v>32454</v>
       </c>
@@ -8280,8 +8965,17 @@
       <c r="C60" s="6" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="15">
+      <c r="E60">
+        <v>786</v>
+      </c>
+      <c r="F60" t="s">
+        <v>764</v>
+      </c>
+      <c r="G60" s="7">
+        <v>32454</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="14">
         <v>7425</v>
       </c>
@@ -8291,8 +8985,17 @@
       <c r="C61" s="6" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="15">
+      <c r="E61">
+        <v>1799</v>
+      </c>
+      <c r="F61" t="s">
+        <v>765</v>
+      </c>
+      <c r="G61" s="14">
+        <v>7425</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="7">
         <v>167024</v>
       </c>
@@ -8301,6 +9004,15 @@
       </c>
       <c r="C62" s="6" t="s">
         <v>767</v>
+      </c>
+      <c r="E62">
+        <v>753</v>
+      </c>
+      <c r="F62" t="s">
+        <v>767</v>
+      </c>
+      <c r="G62" s="7">
+        <v>167024</v>
       </c>
     </row>
   </sheetData>
@@ -15802,7 +16514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -20000,7 +20712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK69"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="N59" sqref="D2:N59"/>
     </sheetView>
   </sheetViews>
@@ -29748,10 +30460,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D58"/>
+      <selection activeCell="C69" sqref="C69:D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -31472,7 +32184,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="2:14">
+    <row r="49" spans="3:14">
       <c r="C49">
         <v>172</v>
       </c>
@@ -31501,7 +32213,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="50" spans="2:14">
+    <row r="50" spans="3:14">
       <c r="C50">
         <v>485</v>
       </c>
@@ -31531,7 +32243,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="51" spans="2:14">
+    <row r="51" spans="3:14">
       <c r="C51">
         <v>1248</v>
       </c>
@@ -31569,7 +32281,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="52" spans="2:14">
+    <row r="52" spans="3:14">
       <c r="C52">
         <v>1272</v>
       </c>
@@ -31598,7 +32310,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="53" spans="2:14">
+    <row r="53" spans="3:14">
       <c r="C53">
         <v>1274</v>
       </c>
@@ -31634,7 +32346,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="54" spans="2:14">
+    <row r="54" spans="3:14">
       <c r="C54">
         <v>1070</v>
       </c>
@@ -31672,7 +32384,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="55" spans="2:14">
+    <row r="55" spans="3:14">
       <c r="C55">
         <v>1325</v>
       </c>
@@ -31710,7 +32422,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="56" spans="2:14">
+    <row r="56" spans="3:14">
       <c r="C56">
         <v>786</v>
       </c>
@@ -31737,7 +32449,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="57" spans="2:14">
+    <row r="57" spans="3:14">
       <c r="C57">
         <v>1799</v>
       </c>
@@ -31775,7 +32487,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="58" spans="2:14">
+    <row r="58" spans="3:14">
       <c r="C58">
         <v>753</v>
       </c>
@@ -31813,36 +32525,500 @@
         <v>330</v>
       </c>
     </row>
-    <row r="59" spans="2:14">
-      <c r="B59" s="16" t="s">
+    <row r="69" spans="3:4">
+      <c r="C69" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4">
+      <c r="C70">
+        <v>51</v>
+      </c>
+      <c r="D70" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4">
+      <c r="C71">
+        <v>1551</v>
+      </c>
+      <c r="D71" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="72" spans="3:4">
+      <c r="C72">
+        <v>1240</v>
+      </c>
+      <c r="D72" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4">
+      <c r="C73">
+        <v>373</v>
+      </c>
+      <c r="D73" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4">
+      <c r="C74">
+        <v>396</v>
+      </c>
+      <c r="D74" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4">
+      <c r="C75">
+        <v>1530</v>
+      </c>
+      <c r="D75" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4">
+      <c r="C76" s="16">
+        <v>1586</v>
+      </c>
+      <c r="D76" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="16">
-        <v>1586</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14">
-      <c r="B60" s="16" t="s">
+    </row>
+    <row r="77" spans="3:4">
+      <c r="C77">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="78" spans="3:4">
+      <c r="C78">
+        <v>1069</v>
+      </c>
+      <c r="D78" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4">
+      <c r="C79" s="16">
+        <v>960</v>
+      </c>
+      <c r="D79" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="C60" s="16">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14">
-      <c r="B61" s="16" t="s">
+    </row>
+    <row r="80" spans="3:4">
+      <c r="C80">
+        <v>1160</v>
+      </c>
+      <c r="D80" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4">
+      <c r="C81">
+        <v>930</v>
+      </c>
+      <c r="D81" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4">
+      <c r="C82">
+        <v>1285</v>
+      </c>
+      <c r="D82" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4">
+      <c r="C83">
+        <v>1026</v>
+      </c>
+      <c r="D83" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4">
+      <c r="C84">
+        <v>622</v>
+      </c>
+      <c r="D84" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4">
+      <c r="C85">
+        <v>1227</v>
+      </c>
+      <c r="D85" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4">
+      <c r="C86">
+        <v>852</v>
+      </c>
+      <c r="D86" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4">
+      <c r="C87">
+        <v>437</v>
+      </c>
+      <c r="D87" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4">
+      <c r="C88">
+        <v>118</v>
+      </c>
+      <c r="D88" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4">
+      <c r="C89">
+        <v>632</v>
+      </c>
+      <c r="D89" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4">
+      <c r="C90">
+        <v>1074</v>
+      </c>
+      <c r="D90" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4">
+      <c r="C91" s="16">
+        <v>721</v>
+      </c>
+      <c r="D91" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="16">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14">
-      <c r="B62" s="16" t="s">
+    </row>
+    <row r="92" spans="3:4">
+      <c r="C92">
+        <v>336</v>
+      </c>
+      <c r="D92" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4">
+      <c r="C93">
+        <v>6</v>
+      </c>
+      <c r="D93" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4">
+      <c r="C94">
+        <v>922</v>
+      </c>
+      <c r="D94" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4">
+      <c r="C95">
+        <v>1143</v>
+      </c>
+      <c r="D95" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4">
+      <c r="C96">
+        <v>1305</v>
+      </c>
+      <c r="D96" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4">
+      <c r="C97">
+        <v>1729</v>
+      </c>
+      <c r="D97" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4">
+      <c r="C98">
+        <v>1580</v>
+      </c>
+      <c r="D98" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4">
+      <c r="C99">
+        <v>1255</v>
+      </c>
+      <c r="D99" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4">
+      <c r="C100" s="16">
+        <v>311</v>
+      </c>
+      <c r="D100" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="C62" s="16">
-        <v>311</v>
+    </row>
+    <row r="101" spans="3:4">
+      <c r="C101">
+        <v>1076</v>
+      </c>
+      <c r="D101" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4">
+      <c r="C102">
+        <v>1814</v>
+      </c>
+      <c r="D102" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4">
+      <c r="C103">
+        <v>717</v>
+      </c>
+      <c r="D103" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4">
+      <c r="C104">
+        <v>1229</v>
+      </c>
+      <c r="D104" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4">
+      <c r="C105">
+        <v>1628</v>
+      </c>
+      <c r="D105" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4">
+      <c r="C106">
+        <v>525</v>
+      </c>
+      <c r="D106" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4">
+      <c r="C107">
+        <v>1274</v>
+      </c>
+      <c r="D107" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4">
+      <c r="C108">
+        <v>999</v>
+      </c>
+      <c r="D108" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4">
+      <c r="C109">
+        <v>475</v>
+      </c>
+      <c r="D109" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4">
+      <c r="C110">
+        <v>46</v>
+      </c>
+      <c r="D110" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4">
+      <c r="C111">
+        <v>1084</v>
+      </c>
+      <c r="D111" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4">
+      <c r="C112">
+        <v>17</v>
+      </c>
+      <c r="D112" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4">
+      <c r="C113">
+        <v>1575</v>
+      </c>
+      <c r="D113" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4">
+      <c r="C114">
+        <v>1798</v>
+      </c>
+      <c r="D114" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="115" spans="3:4">
+      <c r="C115">
+        <v>1000</v>
+      </c>
+      <c r="D115" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="116" spans="3:4">
+      <c r="C116">
+        <v>572</v>
+      </c>
+      <c r="D116" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="117" spans="3:4">
+      <c r="C117">
+        <v>495</v>
+      </c>
+      <c r="D117" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="118" spans="3:4">
+      <c r="C118">
+        <v>117</v>
+      </c>
+      <c r="D118" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="119" spans="3:4">
+      <c r="C119">
+        <v>1826</v>
+      </c>
+      <c r="D119" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="120" spans="3:4">
+      <c r="C120">
+        <v>172</v>
+      </c>
+      <c r="D120" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="121" spans="3:4">
+      <c r="C121">
+        <v>485</v>
+      </c>
+      <c r="D121" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="122" spans="3:4">
+      <c r="C122">
+        <v>1248</v>
+      </c>
+      <c r="D122" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="123" spans="3:4">
+      <c r="C123">
+        <v>1272</v>
+      </c>
+      <c r="D123" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="124" spans="3:4">
+      <c r="C124">
+        <v>972</v>
+      </c>
+      <c r="D124" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="125" spans="3:4">
+      <c r="C125">
+        <v>480</v>
+      </c>
+      <c r="D125" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="126" spans="3:4">
+      <c r="C126">
+        <v>1070</v>
+      </c>
+      <c r="D126" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="127" spans="3:4">
+      <c r="C127">
+        <v>1325</v>
+      </c>
+      <c r="D127" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="128" spans="3:4">
+      <c r="C128">
+        <v>786</v>
+      </c>
+      <c r="D128" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="129" spans="3:4">
+      <c r="C129">
+        <v>1799</v>
+      </c>
+      <c r="D129" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="130" spans="3:4">
+      <c r="C130">
+        <v>753</v>
+      </c>
+      <c r="D130" t="s">
+        <v>767</v>
       </c>
     </row>
   </sheetData>
@@ -31863,7 +33039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K180"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D58" sqref="C1:D58"/>
     </sheetView>
   </sheetViews>
@@ -34533,8 +35709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -37592,6 +38768,7 @@
     <sortCondition ref="C1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>